<commit_message>
SQL Metninde Düzenleme Yaptım
</commit_message>
<xml_diff>
--- a/VERİTABANI DİYAGRAMI.xlsx
+++ b/VERİTABANI DİYAGRAMI.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="97">
   <si>
     <t>Aksiyon</t>
   </si>
@@ -249,9 +249,6 @@
     <t>YrmIDFK</t>
   </si>
   <si>
-    <t>EserlerIDFK</t>
-  </si>
-  <si>
     <t>UyeIDFK</t>
   </si>
   <si>
@@ -306,13 +303,13 @@
     <t>YonetmenIDFK</t>
   </si>
   <si>
-    <t>Izlediklerim(EserlerIDFK)</t>
-  </si>
-  <si>
-    <t>Izlenecekler(EserlerIDFK)</t>
-  </si>
-  <si>
     <t>MovieStallPuani</t>
+  </si>
+  <si>
+    <t>Izlediklerim(EserBilgisiID)</t>
+  </si>
+  <si>
+    <t>Izlenecekler(EserBilgisiID)</t>
   </si>
 </sst>
 </file>
@@ -487,7 +484,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -525,9 +522,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -555,12 +549,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -573,28 +588,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -886,58 +880,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="10.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="12.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" style="3" customWidth="1"/>
+    <col min="1" max="4" width="10.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="15.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" style="3" customWidth="1"/>
     <col min="16" max="17" width="25" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="2.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="16384" width="9.7109375" style="3"/>
+    <col min="23" max="23" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="4.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="2.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="16384" width="9.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:25" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="35"/>
-      <c r="K1" s="29" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="28"/>
+      <c r="K1" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="29"/>
+      <c r="L1" s="22"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
@@ -945,7 +939,7 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>30</v>
       </c>
@@ -980,7 +974,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>1</v>
       </c>
@@ -1015,7 +1009,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -1050,38 +1044,38 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+    <row r="7" spans="1:25" ht="18" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="36"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="30" t="s">
+      <c r="B7" s="29"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="32"/>
-      <c r="I7" s="25" t="s">
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="25"/>
+      <c r="I7" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="20"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="9" t="s">
         <v>25</v>
       </c>
@@ -1094,8 +1088,8 @@
       <c r="G8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="14" t="s">
-        <v>85</v>
+      <c r="I8" s="13" t="s">
+        <v>84</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>61</v>
@@ -1113,7 +1107,7 @@
         <v>63</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P8" s="12" t="s">
         <v>64</v>
@@ -1122,14 +1116,14 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>1</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="6">
         <v>1</v>
       </c>
@@ -1164,14 +1158,14 @@
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
     </row>
-    <row r="10" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>2</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="21"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="6">
         <v>2</v>
       </c>
@@ -1186,14 +1180,14 @@
       </c>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>3</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="6">
         <v>3</v>
       </c>
@@ -1206,25 +1200,25 @@
       <c r="G11" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="I11" s="26" t="s">
+      <c r="I11" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="6">
         <v>4</v>
       </c>
@@ -1237,33 +1231,33 @@
       <c r="G12" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="K12" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="K12" s="12" t="s">
-        <v>89</v>
-      </c>
       <c r="L12" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M12" s="7" t="s">
         <v>8</v>
       </c>
       <c r="N12" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="O12" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="P12" s="12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C13" s="21"/>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="C13" s="20"/>
       <c r="D13" s="6">
         <v>5</v>
       </c>
@@ -1285,8 +1279,8 @@
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C14" s="21"/>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="C14" s="20"/>
       <c r="D14" s="6">
         <v>6</v>
       </c>
@@ -1300,8 +1294,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:25" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C15" s="21"/>
+    <row r="15" spans="1:25" ht="18" x14ac:dyDescent="0.3">
+      <c r="C15" s="20"/>
       <c r="D15" s="6">
         <v>7</v>
       </c>
@@ -1314,19 +1308,19 @@
       <c r="G15" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="I15" s="27" t="s">
+      <c r="I15" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C16" s="21"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="33"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="C16" s="20"/>
       <c r="D16" s="6">
         <v>8</v>
       </c>
@@ -1339,33 +1333,33 @@
       <c r="G16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="16" t="s">
+      <c r="I16" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="J16" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="K16" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="K16" s="12" t="s">
-        <v>92</v>
-      </c>
       <c r="L16" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M16" s="7" t="s">
         <v>8</v>
       </c>
       <c r="N16" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="O16" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="O16" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="P16" s="12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C17" s="21"/>
+    <row r="17" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C17" s="20"/>
       <c r="D17" s="6">
         <v>9</v>
       </c>
@@ -1387,8 +1381,8 @@
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
     </row>
-    <row r="18" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C18" s="21"/>
+    <row r="18" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C18" s="20"/>
       <c r="D18" s="6">
         <v>10</v>
       </c>
@@ -1402,8 +1396,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="3:22" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C19" s="21"/>
+    <row r="19" spans="3:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="C19" s="20"/>
       <c r="D19" s="6">
         <v>11</v>
       </c>
@@ -1416,19 +1410,22 @@
       <c r="G19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="I19" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-    </row>
-    <row r="20" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C20" s="21"/>
+      <c r="I19" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="30"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="30"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="30"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="30"/>
+    </row>
+    <row r="20" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C20" s="20"/>
       <c r="D20" s="6">
         <v>12</v>
       </c>
@@ -1441,27 +1438,42 @@
       <c r="G20" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="I20" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="J20" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L20" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="M20" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="N20" s="19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C21" s="21"/>
+      <c r="I20" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="M20" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="P20" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="R20" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="S20" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C21" s="20"/>
       <c r="D21" s="6">
         <v>13</v>
       </c>
@@ -1480,9 +1492,14 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-    </row>
-    <row r="22" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C22" s="21"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+    </row>
+    <row r="22" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C22" s="20"/>
       <c r="D22" s="6">
         <v>14</v>
       </c>
@@ -1496,8 +1513,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="3:22" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C23" s="21"/>
+    <row r="23" spans="3:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="C23" s="20"/>
       <c r="D23" s="6">
         <v>15</v>
       </c>
@@ -1510,22 +1527,17 @@
       <c r="G23" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="I23" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-    </row>
-    <row r="24" spans="3:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="21"/>
+      <c r="I23" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="35"/>
+    </row>
+    <row r="24" spans="3:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="20"/>
       <c r="D24" s="6">
         <v>16</v>
       </c>
@@ -1539,42 +1551,27 @@
         <v>52</v>
       </c>
       <c r="H24" s="3"/>
-      <c r="I24" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>34</v>
+      <c r="I24" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>76</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="O24" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="P24" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q24" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="R24" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="S24" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C25" s="21"/>
+    </row>
+    <row r="25" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C25" s="20"/>
       <c r="D25" s="6">
         <v>17</v>
       </c>
@@ -1593,14 +1590,9 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
-    </row>
-    <row r="26" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C26" s="21"/>
+    </row>
+    <row r="26" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="C26" s="20"/>
       <c r="D26" s="6">
         <v>18</v>
       </c>
@@ -1614,8 +1606,8 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="3:22" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C27" s="21"/>
+    <row r="27" spans="3:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="C27" s="20"/>
       <c r="D27" s="6">
         <v>19</v>
       </c>
@@ -1628,64 +1620,60 @@
       <c r="G27" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="I27" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
+      <c r="I27" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="34"/>
+      <c r="N27" s="34"/>
+      <c r="O27" s="21"/>
       <c r="V27" s="1"/>
     </row>
-    <row r="28" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="I28" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="J28" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="K28" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="L28" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="M28" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="N28" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="O28" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="I28" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L28" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="M28" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="N28" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="3:22" x14ac:dyDescent="0.3">
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
     </row>
   </sheetData>
   <sortState ref="AC4:AC24">
     <sortCondition ref="AC4"/>
   </sortState>
   <mergeCells count="10">
+    <mergeCell ref="I23:N23"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="D7:G7"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="I23:S23"/>
+    <mergeCell ref="I19:S19"/>
     <mergeCell ref="I7:Q7"/>
     <mergeCell ref="I11:P11"/>
     <mergeCell ref="I15:P15"/>
-    <mergeCell ref="I19:N19"/>
-    <mergeCell ref="I27:O27"/>
+    <mergeCell ref="I27:N27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1"/>

</xml_diff>